<commit_message>
Fix syllabification errors in coding sheets See read-study1_issues-with-syllabification.xlsx, Drive
</commit_message>
<xml_diff>
--- a/materials/reading-ranger/stimuli/passage-error-excels/set-11a/muffins_11g.xlsx
+++ b/materials/reading-ranger/stimuli/passage-error-excels/set-11a/muffins_11g.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="338">
   <si>
     <t xml:space="preserve">Muffins,</t>
   </si>
@@ -748,178 +748,175 @@
     <t xml:space="preserve">ment</t>
   </si>
   <si>
+    <t xml:space="preserve">o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lone;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">po</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">na</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">al</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">less,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thought</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rries,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">late,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">butes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tinct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">er</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ence,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">han</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ture.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ffin's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stenc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">king</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">te</t>
+  </si>
+  <si>
     <t xml:space="preserve">me</t>
-  </si>
-  <si>
-    <t xml:space="preserve">als</t>
-  </si>
-  <si>
-    <t xml:space="preserve">o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fined</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lone;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">po</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">na</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">al</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bound</t>
-  </si>
-  <si>
-    <t xml:space="preserve">less,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thought</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ful</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fused</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rries,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">late,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">butes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tinct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">er</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ence,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">han</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ture.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ffin's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">der,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stenc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">king</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">te</t>
   </si>
   <si>
     <t xml:space="preserve">cu</t>
@@ -1660,7 +1657,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:ZO1003"/>
+  <dimension ref="A1:ZN1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1674,6 +1671,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1997,481 +1995,481 @@
       <c r="EV1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="EW1" s="3"/>
-      <c r="EX1" s="5" t="s">
+      <c r="EW1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="EY1" s="3" t="s">
+      <c r="EX1" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="EY1" s="3"/>
       <c r="EZ1" s="3"/>
-      <c r="FA1" s="3"/>
+      <c r="FA1" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="FB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="FC1" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="FC1" s="3"/>
       <c r="FD1" s="3"/>
       <c r="FE1" s="3"/>
       <c r="FF1" s="3"/>
-      <c r="FG1" s="3"/>
+      <c r="FG1" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="FH1" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="FI1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="FJ1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="FK1" s="3"/>
+      <c r="FJ1" s="3"/>
+      <c r="FK1" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="FL1" s="3" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="FM1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="FN1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="FO1" s="3"/>
-      <c r="FP1" s="4" t="s">
+      <c r="FN1" s="3"/>
+      <c r="FO1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="FQ1" s="3" t="s">
+      <c r="FP1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="FR1" s="3"/>
-      <c r="FS1" s="3" t="s">
+      <c r="FQ1" s="3"/>
+      <c r="FR1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="FT1" s="5" t="s">
+      <c r="FS1" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="FT1" s="5"/>
       <c r="FU1" s="5"/>
-      <c r="FV1" s="5"/>
-      <c r="FW1" s="3" t="s">
+      <c r="FV1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="FX1" s="3"/>
-      <c r="FY1" s="3" t="s">
+      <c r="FW1" s="3"/>
+      <c r="FX1" s="3" t="s">
         <v>81</v>
       </c>
+      <c r="FY1" s="3"/>
       <c r="FZ1" s="3"/>
       <c r="GA1" s="3"/>
-      <c r="GB1" s="3"/>
+      <c r="GB1" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="GC1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="GD1" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="GD1" s="3"/>
       <c r="GE1" s="3"/>
       <c r="GF1" s="3"/>
-      <c r="GG1" s="3"/>
-      <c r="GH1" s="3" t="s">
+      <c r="GG1" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="GH1" s="3"/>
       <c r="GI1" s="3"/>
       <c r="GJ1" s="3"/>
-      <c r="GK1" s="3"/>
+      <c r="GK1" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="GL1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="GM1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="GN1" s="3"/>
+      <c r="GM1" s="3"/>
+      <c r="GN1" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="GO1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="GP1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="GQ1" s="3"/>
-      <c r="GR1" s="4" t="s">
+      <c r="GP1" s="3"/>
+      <c r="GQ1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="GS1" s="5" t="s">
+      <c r="GR1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="GT1" s="5"/>
-      <c r="GU1" s="3" t="s">
+      <c r="GS1" s="5"/>
+      <c r="GT1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="GV1" s="4" t="s">
+      <c r="GU1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="GW1" s="3" t="s">
+      <c r="GV1" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="GW1" s="3"/>
       <c r="GX1" s="3"/>
-      <c r="GY1" s="3"/>
-      <c r="GZ1" s="6" t="s">
+      <c r="GY1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="HA1" s="6"/>
+      <c r="GZ1" s="6"/>
+      <c r="HA1" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="HB1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="HC1" s="3" t="s">
         <v>91</v>
       </c>
+      <c r="HC1" s="3"/>
       <c r="HD1" s="3"/>
-      <c r="HE1" s="3"/>
-      <c r="HF1" s="3" t="s">
+      <c r="HE1" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="HF1" s="3"/>
       <c r="HG1" s="3"/>
-      <c r="HH1" s="3"/>
-      <c r="HI1" s="4" t="s">
+      <c r="HH1" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="HI1" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="HJ1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="HK1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="HL1" s="5" t="s">
+      <c r="HK1" s="5" t="s">
         <v>96</v>
       </c>
+      <c r="HL1" s="5"/>
       <c r="HM1" s="5"/>
-      <c r="HN1" s="5"/>
-      <c r="HO1" s="3" t="s">
+      <c r="HN1" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="HO1" s="3"/>
       <c r="HP1" s="3"/>
-      <c r="HQ1" s="3"/>
+      <c r="HQ1" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="HR1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="HS1" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="HT1" s="3"/>
-      <c r="HU1" s="3" t="s">
+      <c r="HS1" s="3"/>
+      <c r="HT1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="HV1" s="3"/>
-      <c r="HW1" s="3" t="s">
+      <c r="HU1" s="3"/>
+      <c r="HV1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="HX1" s="4" t="s">
+      <c r="HW1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="HY1" s="3" t="s">
+      <c r="HX1" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="HY1" s="3"/>
       <c r="HZ1" s="3"/>
       <c r="IA1" s="3"/>
-      <c r="IB1" s="3"/>
-      <c r="IC1" s="3" t="s">
+      <c r="IB1" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="IC1" s="3"/>
       <c r="ID1" s="3"/>
       <c r="IE1" s="3"/>
-      <c r="IF1" s="3"/>
-      <c r="IG1" s="3" t="s">
+      <c r="IF1" s="3" t="s">
         <v>102</v>
       </c>
+      <c r="IG1" s="3"/>
       <c r="IH1" s="3"/>
-      <c r="II1" s="3"/>
-      <c r="IJ1" s="3" t="s">
+      <c r="II1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="IK1" s="5" t="s">
+      <c r="IJ1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="IL1" s="5"/>
-      <c r="IM1" s="3" t="s">
+      <c r="IK1" s="5"/>
+      <c r="IL1" s="3" t="s">
         <v>103</v>
       </c>
+      <c r="IM1" s="3"/>
       <c r="IN1" s="3"/>
       <c r="IO1" s="3"/>
-      <c r="IP1" s="3"/>
+      <c r="IP1" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="IQ1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="IR1" s="3" t="s">
         <v>104</v>
       </c>
+      <c r="IR1" s="3"/>
       <c r="IS1" s="3"/>
       <c r="IT1" s="3"/>
       <c r="IU1" s="3"/>
-      <c r="IV1" s="3"/>
+      <c r="IV1" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="IW1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="IX1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="IY1" s="3"/>
+      <c r="IX1" s="3"/>
+      <c r="IY1" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="IZ1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="JA1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="JB1" s="3"/>
+      <c r="JA1" s="3"/>
+      <c r="JB1" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="JC1" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="JD1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="JE1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="JF1" s="3"/>
-      <c r="JG1" s="4" t="s">
+      <c r="JE1" s="3"/>
+      <c r="JF1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="JH1" s="3" t="s">
+      <c r="JG1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="JI1" s="5" t="s">
+      <c r="JH1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="JJ1" s="3" t="s">
+      <c r="JI1" s="3" t="s">
         <v>110</v>
       </c>
+      <c r="JJ1" s="3"/>
       <c r="JK1" s="3"/>
-      <c r="JL1" s="3"/>
+      <c r="JL1" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="JM1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="JN1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="JO1" s="3"/>
+      <c r="JN1" s="3"/>
+      <c r="JO1" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="JP1" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="JQ1" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="JR1" s="4" t="s">
         <v>114</v>
       </c>
+      <c r="JR1" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="JS1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="JT1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="JU1" s="3"/>
+      <c r="JT1" s="3"/>
+      <c r="JU1" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="JV1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="JW1" s="3" t="s">
         <v>117</v>
       </c>
+      <c r="JW1" s="3"/>
       <c r="JX1" s="3"/>
       <c r="JY1" s="3"/>
-      <c r="JZ1" s="3"/>
-      <c r="KA1" s="3" t="s">
+      <c r="JZ1" s="3" t="s">
         <v>118</v>
       </c>
+      <c r="KA1" s="3"/>
       <c r="KB1" s="3"/>
-      <c r="KC1" s="3"/>
-      <c r="KD1" s="3" t="s">
+      <c r="KC1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="KE1" s="5" t="s">
+      <c r="KD1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="KF1" s="4" t="s">
+      <c r="KE1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="KG1" s="3" t="s">
+      <c r="KF1" s="3" t="s">
         <v>120</v>
       </c>
+      <c r="KG1" s="3"/>
       <c r="KH1" s="3"/>
-      <c r="KI1" s="3"/>
+      <c r="KI1" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="KJ1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="KK1" s="3" t="s">
         <v>121</v>
       </c>
+      <c r="KK1" s="3"/>
       <c r="KL1" s="3"/>
-      <c r="KM1" s="3"/>
-      <c r="KN1" s="3" t="s">
+      <c r="KM1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="KO1" s="4" t="s">
+      <c r="KN1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="KP1" s="3" t="s">
+      <c r="KO1" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="KP1" s="3"/>
       <c r="KQ1" s="3"/>
       <c r="KR1" s="3"/>
-      <c r="KS1" s="3"/>
-      <c r="KT1" s="4" t="s">
+      <c r="KS1" s="4" t="s">
         <v>113</v>
       </c>
+      <c r="KT1" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="KU1" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="KV1" s="3" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="KW1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="KX1" s="3" t="s">
         <v>126</v>
       </c>
+      <c r="KX1" s="3"/>
       <c r="KY1" s="3"/>
-      <c r="KZ1" s="3"/>
-      <c r="LA1" s="3" t="s">
+      <c r="KZ1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="LB1" s="5" t="s">
+      <c r="LA1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="LC1" s="3" t="s">
+      <c r="LB1" s="3" t="s">
         <v>127</v>
       </c>
+      <c r="LC1" s="3"/>
       <c r="LD1" s="3"/>
       <c r="LE1" s="3"/>
-      <c r="LF1" s="3"/>
-      <c r="LG1" s="3" t="s">
+      <c r="LF1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="LH1" s="3"/>
-      <c r="LI1" s="3" t="s">
+      <c r="LG1" s="3"/>
+      <c r="LH1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="LJ1" s="3"/>
+      <c r="LI1" s="3"/>
+      <c r="LJ1" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="LK1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="LL1" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="LM1" s="3"/>
-      <c r="LN1" s="3" t="s">
+      <c r="LL1" s="3"/>
+      <c r="LM1" s="3" t="s">
         <v>131</v>
       </c>
+      <c r="LN1" s="3"/>
       <c r="LO1" s="3"/>
       <c r="LP1" s="3"/>
-      <c r="LQ1" s="3"/>
+      <c r="LQ1" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="LR1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="LS1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="LT1" s="3"/>
-      <c r="LU1" s="4" t="s">
+      <c r="LS1" s="3"/>
+      <c r="LT1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="LV1" s="3" t="s">
+      <c r="LU1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="LW1" s="3"/>
+      <c r="LV1" s="3"/>
+      <c r="LW1" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="LX1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="LY1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="LZ1" s="5" t="s">
+      <c r="LY1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="MA1" s="5"/>
-      <c r="MB1" s="3" t="s">
+      <c r="LZ1" s="5"/>
+      <c r="MA1" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="MB1" s="3"/>
       <c r="MC1" s="3"/>
-      <c r="MD1" s="3"/>
-      <c r="ME1" s="4" t="s">
+      <c r="MD1" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="ME1" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="MF1" s="3" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="MG1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="MH1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="MI1" s="3"/>
-      <c r="MJ1" s="3" t="s">
+      <c r="MH1" s="3"/>
+      <c r="MI1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="MK1" s="3"/>
-      <c r="ML1" s="3" t="s">
+      <c r="MJ1" s="3"/>
+      <c r="MK1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="MM1" s="3"/>
+      <c r="ML1" s="3"/>
+      <c r="MM1" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="MN1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="MO1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="MP1" s="3"/>
+      <c r="MO1" s="3"/>
+      <c r="MP1" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="MQ1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="MR1" s="3" t="s">
         <v>142</v>
       </c>
+      <c r="MR1" s="3"/>
       <c r="MS1" s="3"/>
-      <c r="MT1" s="3"/>
-      <c r="MU1" s="3" t="s">
+      <c r="MT1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="MV1" s="3"/>
-      <c r="MW1" s="3" t="s">
+      <c r="MU1" s="3"/>
+      <c r="MV1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="MX1" s="5" t="s">
+      <c r="MW1" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="MY1" s="3" t="s">
+      <c r="MX1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="MZ1" s="3"/>
-      <c r="NA1" s="3" t="s">
+      <c r="MY1" s="3"/>
+      <c r="MZ1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="NB1" s="3"/>
+      <c r="NA1" s="3"/>
+      <c r="NB1" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="NC1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="ND1" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="NE1" s="4" t="s">
+      <c r="ND1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="NF1" s="3" t="s">
+      <c r="NE1" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="NG1" s="3"/>
-      <c r="NH1" s="3" t="s">
+      <c r="NF1" s="3"/>
+      <c r="NG1" s="3" t="s">
         <v>149</v>
       </c>
+      <c r="NH1" s="3"/>
       <c r="NI1" s="3"/>
-      <c r="NJ1" s="3"/>
-      <c r="NK1" s="3" t="s">
+      <c r="NJ1" s="3" t="s">
         <v>150</v>
       </c>
+      <c r="NK1" s="3"/>
       <c r="NL1" s="3"/>
       <c r="NM1" s="3"/>
-      <c r="NN1" s="3"/>
-      <c r="NO1" s="3" t="s">
+      <c r="NN1" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="NP1" s="3"/>
-      <c r="NQ1" s="4"/>
+      <c r="NO1" s="3"/>
+      <c r="NP1" s="4"/>
+      <c r="NQ1" s="3"/>
       <c r="NR1" s="3"/>
       <c r="NS1" s="3"/>
       <c r="NT1" s="3"/>
@@ -2479,15 +2477,15 @@
       <c r="NV1" s="3"/>
       <c r="NW1" s="3"/>
       <c r="NX1" s="3"/>
-      <c r="NY1" s="3"/>
-      <c r="NZ1" s="4"/>
+      <c r="NY1" s="4"/>
+      <c r="NZ1" s="3"/>
       <c r="OA1" s="3"/>
       <c r="OB1" s="3"/>
       <c r="OC1" s="3"/>
       <c r="OD1" s="3"/>
-      <c r="OE1" s="3"/>
+      <c r="OE1" s="4"/>
       <c r="OF1" s="4"/>
-      <c r="OG1" s="4"/>
+      <c r="OG1" s="3"/>
       <c r="OH1" s="3"/>
       <c r="OI1" s="3"/>
       <c r="OJ1" s="3"/>
@@ -2498,110 +2496,110 @@
       <c r="OO1" s="3"/>
       <c r="OP1" s="3"/>
       <c r="OQ1" s="3"/>
-      <c r="OR1" s="3"/>
+      <c r="OR1" s="4"/>
       <c r="OS1" s="4"/>
       <c r="OT1" s="4"/>
       <c r="OU1" s="4"/>
-      <c r="OV1" s="4"/>
+      <c r="OV1" s="3"/>
       <c r="OW1" s="3"/>
       <c r="OX1" s="3"/>
       <c r="OY1" s="3"/>
       <c r="OZ1" s="3"/>
-      <c r="PA1" s="3"/>
+      <c r="PA1" s="4"/>
       <c r="PB1" s="4"/>
-      <c r="PC1" s="4"/>
+      <c r="PC1" s="3"/>
       <c r="PD1" s="3"/>
       <c r="PE1" s="3"/>
       <c r="PF1" s="3"/>
-      <c r="PG1" s="3"/>
+      <c r="PG1" s="4"/>
       <c r="PH1" s="4"/>
       <c r="PI1" s="4"/>
-      <c r="PJ1" s="4"/>
+      <c r="PJ1" s="3"/>
       <c r="PK1" s="3"/>
-      <c r="PL1" s="3"/>
-      <c r="PM1" s="4"/>
+      <c r="PL1" s="4"/>
+      <c r="PM1" s="3"/>
       <c r="PN1" s="3"/>
       <c r="PO1" s="3"/>
-      <c r="PP1" s="3"/>
-      <c r="PQ1" s="4"/>
+      <c r="PP1" s="4"/>
+      <c r="PQ1" s="3"/>
       <c r="PR1" s="3"/>
-      <c r="PS1" s="3"/>
+      <c r="PS1" s="4"/>
       <c r="PT1" s="4"/>
       <c r="PU1" s="4"/>
-      <c r="PV1" s="4"/>
+      <c r="PV1" s="3"/>
       <c r="PW1" s="3"/>
       <c r="PX1" s="3"/>
-      <c r="PY1" s="3"/>
+      <c r="PY1" s="4"/>
       <c r="PZ1" s="4"/>
-      <c r="QA1" s="4"/>
+      <c r="QA1" s="3"/>
       <c r="QB1" s="3"/>
       <c r="QC1" s="3"/>
       <c r="QD1" s="3"/>
       <c r="QE1" s="3"/>
       <c r="QF1" s="3"/>
-      <c r="QG1" s="3"/>
+      <c r="QG1" s="4"/>
       <c r="QH1" s="4"/>
-      <c r="QI1" s="4"/>
+      <c r="QI1" s="3"/>
       <c r="QJ1" s="3"/>
-      <c r="QK1" s="3"/>
-      <c r="QL1" s="4"/>
+      <c r="QK1" s="4"/>
+      <c r="QL1" s="3"/>
       <c r="QM1" s="3"/>
-      <c r="QN1" s="3"/>
-      <c r="QO1" s="4"/>
+      <c r="QN1" s="4"/>
+      <c r="QO1" s="3"/>
       <c r="QP1" s="3"/>
       <c r="QQ1" s="3"/>
       <c r="QR1" s="3"/>
-      <c r="QS1" s="3"/>
+      <c r="QS1" s="4"/>
       <c r="QT1" s="4"/>
-      <c r="QU1" s="4"/>
+      <c r="QU1" s="3"/>
       <c r="QV1" s="3"/>
       <c r="QW1" s="3"/>
-      <c r="QX1" s="3"/>
+      <c r="QX1" s="4"/>
       <c r="QY1" s="4"/>
       <c r="QZ1" s="4"/>
       <c r="RA1" s="4"/>
-      <c r="RB1" s="4"/>
+      <c r="RB1" s="3"/>
       <c r="RC1" s="3"/>
       <c r="RD1" s="3"/>
       <c r="RE1" s="3"/>
-      <c r="RF1" s="3"/>
-      <c r="RG1" s="4"/>
+      <c r="RF1" s="4"/>
+      <c r="RG1" s="3"/>
       <c r="RH1" s="3"/>
       <c r="RI1" s="3"/>
       <c r="RJ1" s="3"/>
-      <c r="RK1" s="3"/>
+      <c r="RK1" s="4"/>
       <c r="RL1" s="4"/>
-      <c r="RM1" s="4"/>
+      <c r="RM1" s="3"/>
       <c r="RN1" s="3"/>
-      <c r="RO1" s="3"/>
+      <c r="RO1" s="4"/>
       <c r="RP1" s="4"/>
       <c r="RQ1" s="4"/>
       <c r="RR1" s="4"/>
-      <c r="RS1" s="4"/>
+      <c r="RS1" s="3"/>
       <c r="RT1" s="3"/>
       <c r="RU1" s="3"/>
       <c r="RV1" s="3"/>
       <c r="RW1" s="3"/>
-      <c r="RX1" s="3"/>
-      <c r="RY1" s="4"/>
+      <c r="RX1" s="4"/>
+      <c r="RY1" s="3"/>
       <c r="RZ1" s="3"/>
       <c r="SA1" s="3"/>
-      <c r="SB1" s="3"/>
-      <c r="SC1" s="4"/>
+      <c r="SB1" s="4"/>
+      <c r="SC1" s="3"/>
       <c r="SD1" s="3"/>
       <c r="SE1" s="3"/>
-      <c r="SF1" s="3"/>
-      <c r="SG1" s="4"/>
+      <c r="SF1" s="4"/>
+      <c r="SG1" s="3"/>
       <c r="SH1" s="3"/>
-      <c r="SI1" s="3"/>
-      <c r="SJ1" s="4"/>
+      <c r="SI1" s="4"/>
+      <c r="SJ1" s="3"/>
       <c r="SK1" s="3"/>
       <c r="SL1" s="3"/>
       <c r="SM1" s="3"/>
       <c r="SN1" s="3"/>
       <c r="SO1" s="3"/>
-      <c r="SP1" s="3"/>
-      <c r="SQ1" s="4"/>
+      <c r="SP1" s="4"/>
+      <c r="SQ1" s="3"/>
       <c r="SR1" s="3"/>
       <c r="SS1" s="3"/>
       <c r="ST1" s="3"/>
@@ -2612,9 +2610,9 @@
       <c r="SY1" s="3"/>
       <c r="SZ1" s="3"/>
       <c r="TA1" s="3"/>
-      <c r="TB1" s="3"/>
+      <c r="TB1" s="4"/>
       <c r="TC1" s="4"/>
-      <c r="TD1" s="4"/>
+      <c r="TD1" s="3"/>
       <c r="TE1" s="3"/>
       <c r="TF1" s="3"/>
       <c r="TG1" s="3"/>
@@ -2624,7 +2622,7 @@
       <c r="TK1" s="3"/>
       <c r="TL1" s="3"/>
       <c r="TM1" s="3"/>
-      <c r="TN1" s="3"/>
+      <c r="TN1" s="4"/>
       <c r="TO1" s="4"/>
       <c r="TP1" s="4"/>
       <c r="TQ1" s="4"/>
@@ -2781,7 +2779,6 @@
       <c r="ZL1" s="4"/>
       <c r="ZM1" s="4"/>
       <c r="ZN1" s="4"/>
-      <c r="ZO1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
@@ -3236,523 +3233,523 @@
         <v>25</v>
       </c>
       <c r="EV2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="EW2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="EX2" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="EW2" s="8" t="s">
+      <c r="EY2" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="EX2" s="9" t="s">
+      <c r="EZ2" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="FA2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="FB2" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="FC2" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="FD2" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="FE2" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="FF2" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="FG2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="FH2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="FI2" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="FJ2" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="FK2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="FL2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="FM2" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="FN2" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="FO2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="FP2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="FQ2" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="FR2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="FS2" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="FT2" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="FU2" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="FV2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="FW2" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="FX2" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="FY2" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="FZ2" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="GA2" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="GB2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="EY2" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="EZ2" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="FA2" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="FB2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="FC2" s="8" t="s">
+      <c r="GC2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="GD2" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="GE2" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="GF2" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="GG2" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="GH2" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="GI2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="GJ2" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="GK2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="GL2" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="GM2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="GN2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="GO2" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="GP2" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="GQ2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="GR2" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="GS2" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="GT2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="GU2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="GV2" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="GW2" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="GX2" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="GY2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="GZ2" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="HA2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="HB2" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="HC2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="HD2" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="HE2" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="HF2" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="HG2" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="HH2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="HI2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="HJ2" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="HK2" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="HL2" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="HM2" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="HN2" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="HO2" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="HP2" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="HQ2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="HR2" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="HS2" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="HT2" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="HU2" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="HV2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="HW2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="HX2" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="HY2" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="HZ2" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="IA2" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="IB2" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="IC2" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="ID2" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="IE2" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="IF2" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="IG2" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="IH2" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="II2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="IJ2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="IK2" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="IL2" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="IM2" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="IN2" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="IO2" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="IP2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="IQ2" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="IR2" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="FD2" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="FE2" s="8" t="s">
+      <c r="IS2" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="IT2" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="IU2" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="IV2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="IW2" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="IX2" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="IY2" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="IZ2" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="JA2" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="JB2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="JC2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="JD2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="JE2" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="JF2" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="JG2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="JH2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="JI2" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="JJ2" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="JK2" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="JL2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="JM2" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="JN2" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="JO2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="JP2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="JQ2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="JR2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="JS2" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="JT2" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="JU2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="JV2" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="JW2" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="JX2" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="JY2" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="JZ2" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="KA2" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="KB2" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="KC2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="KD2" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="KE2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="KF2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="KG2" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="KH2" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="KI2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="KJ2" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="KK2" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="KL2" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="KM2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="KN2" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="KO2" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="KP2" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="KQ2" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="KR2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="KS2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="KT2" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="KU2" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="KV2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="KW2" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="KX2" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="KY2" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="KZ2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="LA2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="LB2" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="LC2" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="FF2" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="FG2" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="FH2" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="FI2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="FJ2" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="FK2" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="FL2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="FM2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="FN2" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="FO2" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="FP2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="FQ2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="FR2" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="FS2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="FT2" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="FU2" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="FV2" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="FW2" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="FX2" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="FY2" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="FZ2" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="GA2" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="GB2" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="GC2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="GD2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="GE2" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="GF2" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="GG2" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="GH2" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="GI2" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="GJ2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="GK2" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="GL2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="GM2" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="GN2" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="GO2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="GP2" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="GQ2" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="GR2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="GS2" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="GT2" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="GU2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="GV2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="GW2" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="GX2" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="GY2" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="GZ2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="HA2" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="HB2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="HC2" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="HD2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="HE2" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="HF2" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="HG2" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="HH2" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="HI2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="HJ2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="HK2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="HL2" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="HM2" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="HN2" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="HO2" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="HP2" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="HQ2" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="HR2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="HS2" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="HT2" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="HU2" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="HV2" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="HW2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="HX2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="HY2" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="HZ2" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="IA2" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="IB2" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="IC2" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="ID2" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="IE2" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="IF2" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="IG2" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="IH2" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="II2" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="IJ2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="IK2" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="IL2" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="IM2" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="IN2" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="IO2" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="IP2" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="IQ2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="IR2" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="IS2" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="IT2" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="IU2" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="IV2" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="IW2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="IX2" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="IY2" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="IZ2" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="JA2" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="JB2" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="JC2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="JD2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="JE2" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="JF2" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="JG2" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="JH2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="JI2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="JJ2" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="JK2" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="JL2" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="JM2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="JN2" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="JO2" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="JP2" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="JQ2" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="JR2" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="JS2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="JT2" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="JU2" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="JV2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="JW2" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="JX2" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="JY2" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="JZ2" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="KA2" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="KB2" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="KC2" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="KD2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="KE2" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="KF2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="KG2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="KH2" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="KI2" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="KJ2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="KK2" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="KL2" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="KM2" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="KN2" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="KO2" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="KP2" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="KQ2" s="8" t="s">
+      <c r="LD2" s="8" t="s">
         <v>299</v>
-      </c>
-      <c r="KR2" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="KS2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="KT2" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="KU2" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="KV2" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="KW2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="KX2" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="KY2" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="KZ2" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="LA2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="LB2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="LC2" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="LD2" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="LE2" s="8" t="s">
         <v>300</v>
       </c>
       <c r="LF2" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="LG2" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="LH2" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="LG2" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="LH2" s="8" t="s">
-        <v>296</v>
       </c>
       <c r="LI2" s="8" t="s">
         <v>302</v>
       </c>
       <c r="LJ2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="LK2" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="LL2" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="LK2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="LL2" s="8" t="s">
-        <v>188</v>
       </c>
       <c r="LM2" s="8" t="s">
         <v>304</v>
@@ -3761,157 +3758,157 @@
         <v>305</v>
       </c>
       <c r="LO2" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="LP2" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="LP2" s="8" t="s">
-        <v>244</v>
-      </c>
       <c r="LQ2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="LR2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="LS2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="LT2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="LU2" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="LV2" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="LR2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="LS2" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="LT2" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="LU2" s="8" t="s">
+      <c r="LW2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="LX2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="LY2" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="LZ2" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="MA2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="MB2" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="MC2" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="MD2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="ME2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="MF2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="LV2" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="LW2" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="LX2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="LY2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="LZ2" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="MA2" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="MB2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="MC2" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="MD2" s="8" t="s">
+      <c r="MG2" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="ME2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="MF2" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="MG2" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="MH2" s="8" t="s">
         <v>311</v>
       </c>
       <c r="MI2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="MJ2" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="MJ2" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="MK2" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="ML2" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="ML2" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="MM2" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="MN2" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="MN2" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="MO2" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="MP2" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="MQ2" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="MR2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="MS2" s="8" t="s">
         <v>315</v>
-      </c>
-      <c r="MP2" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="MQ2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="MR2" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="MS2" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="MT2" s="8" t="s">
         <v>316</v>
       </c>
       <c r="MU2" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="MV2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="MW2" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="MX2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="MY2" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="MV2" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="MW2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="MX2" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="MY2" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="MZ2" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="NA2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="NB2" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="NC2" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="ND2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="NE2" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="NA2" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="NB2" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="NC2" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="ND2" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="NE2" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="NF2" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="NG2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="NH2" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="NG2" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="NH2" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="NI2" s="1" t="s">
         <v>320</v>
       </c>
       <c r="NJ2" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="NK2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="NL2" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="NM2" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="NK2" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="NL2" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="NM2" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="NN2" s="1" t="s">
         <v>322</v>
@@ -3919,13 +3916,10 @@
       <c r="NO2" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="NP2" s="1" t="s">
-        <v>324</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B3" s="11" t="n">
         <v>0</v>
@@ -4380,10 +4374,10 @@
       <c r="EV3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX3" s="12" t="n">
+      <c r="EW3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY3" s="11" t="n">
@@ -4452,10 +4446,10 @@
       <c r="FT3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV3" s="12" t="n">
+      <c r="FU3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW3" s="11" t="n">
@@ -4524,10 +4518,10 @@
       <c r="GR3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT3" s="12" t="n">
+      <c r="GS3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU3" s="11" t="n">
@@ -4584,10 +4578,10 @@
       <c r="HL3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN3" s="12" t="n">
+      <c r="HM3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO3" s="11" t="n">
@@ -4656,10 +4650,10 @@
       <c r="IJ3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL3" s="12" t="n">
+      <c r="IK3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM3" s="11" t="n">
@@ -4725,10 +4719,10 @@
       <c r="JG3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI3" s="12" t="n">
+      <c r="JH3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ3" s="11" t="n">
@@ -4791,10 +4785,10 @@
       <c r="KC3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE3" s="12" t="n">
+      <c r="KD3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF3" s="11" t="n">
@@ -4860,10 +4854,10 @@
       <c r="KZ3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB3" s="12" t="n">
+      <c r="LA3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC3" s="11" t="n">
@@ -4935,10 +4929,10 @@
       <c r="LY3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA3" s="12" t="n">
+      <c r="LZ3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB3" s="11" t="n">
@@ -5004,10 +4998,10 @@
       <c r="MV3" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX3" s="12" t="n">
+      <c r="MW3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX3" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY3" s="11" t="n">
@@ -5059,15 +5053,12 @@
         <v>0</v>
       </c>
       <c r="NO3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP3" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B4" s="11" t="n">
         <v>0</v>
@@ -5522,10 +5513,10 @@
       <c r="EV4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX4" s="12" t="n">
+      <c r="EW4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY4" s="11" t="n">
@@ -5594,10 +5585,10 @@
       <c r="FT4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV4" s="12" t="n">
+      <c r="FU4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW4" s="11" t="n">
@@ -5666,10 +5657,10 @@
       <c r="GR4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT4" s="12" t="n">
+      <c r="GS4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU4" s="11" t="n">
@@ -5726,10 +5717,10 @@
       <c r="HL4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN4" s="12" t="n">
+      <c r="HM4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO4" s="11" t="n">
@@ -5798,10 +5789,10 @@
       <c r="IJ4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL4" s="12" t="n">
+      <c r="IK4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM4" s="11" t="n">
@@ -5867,10 +5858,10 @@
       <c r="JG4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI4" s="12" t="n">
+      <c r="JH4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ4" s="11" t="n">
@@ -5933,10 +5924,10 @@
       <c r="KC4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE4" s="12" t="n">
+      <c r="KD4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF4" s="11" t="n">
@@ -6002,10 +5993,10 @@
       <c r="KZ4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB4" s="12" t="n">
+      <c r="LA4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC4" s="11" t="n">
@@ -6077,10 +6068,10 @@
       <c r="LY4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA4" s="12" t="n">
+      <c r="LZ4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB4" s="11" t="n">
@@ -6146,10 +6137,10 @@
       <c r="MV4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX4" s="12" t="n">
+      <c r="MW4" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX4" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY4" s="11" t="n">
@@ -6201,15 +6192,12 @@
         <v>0</v>
       </c>
       <c r="NO4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP4" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5" s="11" t="n">
         <v>0</v>
@@ -6664,10 +6652,10 @@
       <c r="EV5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX5" s="12" t="n">
+      <c r="EW5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY5" s="11" t="n">
@@ -6736,10 +6724,10 @@
       <c r="FT5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV5" s="12" t="n">
+      <c r="FU5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW5" s="11" t="n">
@@ -6808,10 +6796,10 @@
       <c r="GR5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT5" s="12" t="n">
+      <c r="GS5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU5" s="11" t="n">
@@ -6868,10 +6856,10 @@
       <c r="HL5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN5" s="12" t="n">
+      <c r="HM5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO5" s="11" t="n">
@@ -6940,10 +6928,10 @@
       <c r="IJ5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL5" s="12" t="n">
+      <c r="IK5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM5" s="11" t="n">
@@ -7009,10 +6997,10 @@
       <c r="JG5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI5" s="12" t="n">
+      <c r="JH5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ5" s="11" t="n">
@@ -7075,10 +7063,10 @@
       <c r="KC5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE5" s="12" t="n">
+      <c r="KD5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF5" s="11" t="n">
@@ -7144,10 +7132,10 @@
       <c r="KZ5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB5" s="12" t="n">
+      <c r="LA5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC5" s="11" t="n">
@@ -7219,10 +7207,10 @@
       <c r="LY5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA5" s="12" t="n">
+      <c r="LZ5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB5" s="11" t="n">
@@ -7288,10 +7276,10 @@
       <c r="MV5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX5" s="12" t="n">
+      <c r="MW5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX5" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY5" s="11" t="n">
@@ -7343,15 +7331,12 @@
         <v>0</v>
       </c>
       <c r="NO5" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP5" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="15" t="n">
         <v>0</v>
@@ -7806,10 +7791,10 @@
       <c r="EV6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="EW6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX6" s="16" t="n">
+      <c r="EW6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="EY6" s="15" t="n">
@@ -7878,10 +7863,10 @@
       <c r="FT6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="FU6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV6" s="16" t="n">
+      <c r="FU6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="FW6" s="15" t="n">
@@ -7950,10 +7935,10 @@
       <c r="GR6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="GS6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT6" s="16" t="n">
+      <c r="GS6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="GU6" s="15" t="n">
@@ -8010,10 +7995,10 @@
       <c r="HL6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="HM6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN6" s="16" t="n">
+      <c r="HM6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="HO6" s="15" t="n">
@@ -8082,10 +8067,10 @@
       <c r="IJ6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="IK6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL6" s="16" t="n">
+      <c r="IK6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="IM6" s="15" t="n">
@@ -8151,10 +8136,10 @@
       <c r="JG6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="JH6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI6" s="16" t="n">
+      <c r="JH6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="JJ6" s="15" t="n">
@@ -8217,10 +8202,10 @@
       <c r="KC6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="KD6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE6" s="16" t="n">
+      <c r="KD6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="KF6" s="15" t="n">
@@ -8286,10 +8271,10 @@
       <c r="KZ6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="LA6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB6" s="16" t="n">
+      <c r="LA6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="LC6" s="15" t="n">
@@ -8361,10 +8346,10 @@
       <c r="LY6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="LZ6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA6" s="16" t="n">
+      <c r="LZ6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="MB6" s="15" t="n">
@@ -8430,10 +8415,10 @@
       <c r="MV6" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="MW6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX6" s="16" t="n">
+      <c r="MW6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="MY6" s="15" t="n">
@@ -8485,15 +8470,12 @@
         <v>0</v>
       </c>
       <c r="NO6" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP6" s="15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7" s="11" t="n">
         <v>0</v>
@@ -8948,10 +8930,10 @@
       <c r="EV7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX7" s="12" t="n">
+      <c r="EW7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY7" s="11" t="n">
@@ -9020,10 +9002,10 @@
       <c r="FT7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV7" s="12" t="n">
+      <c r="FU7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW7" s="11" t="n">
@@ -9092,10 +9074,10 @@
       <c r="GR7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT7" s="12" t="n">
+      <c r="GS7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU7" s="11" t="n">
@@ -9152,10 +9134,10 @@
       <c r="HL7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN7" s="12" t="n">
+      <c r="HM7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO7" s="11" t="n">
@@ -9224,10 +9206,10 @@
       <c r="IJ7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL7" s="12" t="n">
+      <c r="IK7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM7" s="11" t="n">
@@ -9293,10 +9275,10 @@
       <c r="JG7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI7" s="12" t="n">
+      <c r="JH7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ7" s="11" t="n">
@@ -9359,10 +9341,10 @@
       <c r="KC7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE7" s="12" t="n">
+      <c r="KD7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF7" s="11" t="n">
@@ -9428,10 +9410,10 @@
       <c r="KZ7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB7" s="12" t="n">
+      <c r="LA7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC7" s="11" t="n">
@@ -9503,10 +9485,10 @@
       <c r="LY7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA7" s="12" t="n">
+      <c r="LZ7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB7" s="11" t="n">
@@ -9572,10 +9554,10 @@
       <c r="MV7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX7" s="12" t="n">
+      <c r="MW7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX7" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY7" s="11" t="n">
@@ -9627,15 +9609,12 @@
         <v>0</v>
       </c>
       <c r="NO7" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP7" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B8" s="11" t="n">
         <v>0</v>
@@ -10090,10 +10069,10 @@
       <c r="EV8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX8" s="12" t="n">
+      <c r="EW8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY8" s="11" t="n">
@@ -10162,10 +10141,10 @@
       <c r="FT8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV8" s="12" t="n">
+      <c r="FU8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW8" s="11" t="n">
@@ -10234,10 +10213,10 @@
       <c r="GR8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT8" s="12" t="n">
+      <c r="GS8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU8" s="11" t="n">
@@ -10294,10 +10273,10 @@
       <c r="HL8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN8" s="12" t="n">
+      <c r="HM8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO8" s="11" t="n">
@@ -10366,10 +10345,10 @@
       <c r="IJ8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL8" s="12" t="n">
+      <c r="IK8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM8" s="11" t="n">
@@ -10435,10 +10414,10 @@
       <c r="JG8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI8" s="12" t="n">
+      <c r="JH8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ8" s="11" t="n">
@@ -10501,10 +10480,10 @@
       <c r="KC8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE8" s="12" t="n">
+      <c r="KD8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF8" s="11" t="n">
@@ -10570,10 +10549,10 @@
       <c r="KZ8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB8" s="12" t="n">
+      <c r="LA8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC8" s="11" t="n">
@@ -10645,10 +10624,10 @@
       <c r="LY8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA8" s="12" t="n">
+      <c r="LZ8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB8" s="11" t="n">
@@ -10714,10 +10693,10 @@
       <c r="MV8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX8" s="12" t="n">
+      <c r="MW8" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX8" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY8" s="11" t="n">
@@ -10769,15 +10748,12 @@
         <v>0</v>
       </c>
       <c r="NO8" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP8" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B9" s="11" t="n">
         <v>0</v>
@@ -11232,10 +11208,10 @@
       <c r="EV9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX9" s="12" t="n">
+      <c r="EW9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY9" s="11" t="n">
@@ -11304,10 +11280,10 @@
       <c r="FT9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV9" s="12" t="n">
+      <c r="FU9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW9" s="11" t="n">
@@ -11376,10 +11352,10 @@
       <c r="GR9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT9" s="12" t="n">
+      <c r="GS9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU9" s="11" t="n">
@@ -11436,10 +11412,10 @@
       <c r="HL9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN9" s="12" t="n">
+      <c r="HM9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO9" s="11" t="n">
@@ -11508,10 +11484,10 @@
       <c r="IJ9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL9" s="12" t="n">
+      <c r="IK9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM9" s="11" t="n">
@@ -11577,10 +11553,10 @@
       <c r="JG9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI9" s="12" t="n">
+      <c r="JH9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ9" s="11" t="n">
@@ -11643,10 +11619,10 @@
       <c r="KC9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE9" s="12" t="n">
+      <c r="KD9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF9" s="11" t="n">
@@ -11712,10 +11688,10 @@
       <c r="KZ9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB9" s="12" t="n">
+      <c r="LA9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC9" s="11" t="n">
@@ -11787,10 +11763,10 @@
       <c r="LY9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA9" s="12" t="n">
+      <c r="LZ9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB9" s="11" t="n">
@@ -11856,10 +11832,10 @@
       <c r="MV9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX9" s="12" t="n">
+      <c r="MW9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX9" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY9" s="11" t="n">
@@ -11911,15 +11887,12 @@
         <v>0</v>
       </c>
       <c r="NO9" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP9" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B10" s="11" t="n">
         <v>0</v>
@@ -12374,10 +12347,10 @@
       <c r="EV10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX10" s="12" t="n">
+      <c r="EW10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY10" s="11" t="n">
@@ -12446,10 +12419,10 @@
       <c r="FT10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV10" s="12" t="n">
+      <c r="FU10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW10" s="11" t="n">
@@ -12518,10 +12491,10 @@
       <c r="GR10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT10" s="12" t="n">
+      <c r="GS10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU10" s="11" t="n">
@@ -12578,10 +12551,10 @@
       <c r="HL10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN10" s="12" t="n">
+      <c r="HM10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO10" s="11" t="n">
@@ -12650,10 +12623,10 @@
       <c r="IJ10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL10" s="12" t="n">
+      <c r="IK10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM10" s="11" t="n">
@@ -12719,10 +12692,10 @@
       <c r="JG10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI10" s="12" t="n">
+      <c r="JH10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ10" s="11" t="n">
@@ -12785,10 +12758,10 @@
       <c r="KC10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE10" s="12" t="n">
+      <c r="KD10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF10" s="11" t="n">
@@ -12854,10 +12827,10 @@
       <c r="KZ10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB10" s="12" t="n">
+      <c r="LA10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC10" s="11" t="n">
@@ -12929,10 +12902,10 @@
       <c r="LY10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA10" s="12" t="n">
+      <c r="LZ10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB10" s="11" t="n">
@@ -12998,10 +12971,10 @@
       <c r="MV10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX10" s="12" t="n">
+      <c r="MW10" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX10" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY10" s="11" t="n">
@@ -13053,15 +13026,12 @@
         <v>0</v>
       </c>
       <c r="NO10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP10" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" s="21" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B11" s="19" t="n">
         <v>0</v>
@@ -13516,10 +13486,10 @@
       <c r="EV11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="EW11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX11" s="20" t="n">
+      <c r="EW11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="EY11" s="19" t="n">
@@ -13588,10 +13558,10 @@
       <c r="FT11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="FU11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV11" s="20" t="n">
+      <c r="FU11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="FW11" s="19" t="n">
@@ -13660,10 +13630,10 @@
       <c r="GR11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="GS11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT11" s="20" t="n">
+      <c r="GS11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="GU11" s="19" t="n">
@@ -13720,10 +13690,10 @@
       <c r="HL11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="HM11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN11" s="20" t="n">
+      <c r="HM11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="HO11" s="19" t="n">
@@ -13792,10 +13762,10 @@
       <c r="IJ11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="IK11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL11" s="20" t="n">
+      <c r="IK11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="IM11" s="19" t="n">
@@ -13861,10 +13831,10 @@
       <c r="JG11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="JH11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI11" s="20" t="n">
+      <c r="JH11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="JJ11" s="19" t="n">
@@ -13927,10 +13897,10 @@
       <c r="KC11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="KD11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE11" s="20" t="n">
+      <c r="KD11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="KF11" s="19" t="n">
@@ -13996,10 +13966,10 @@
       <c r="KZ11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="LA11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB11" s="20" t="n">
+      <c r="LA11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="LC11" s="19" t="n">
@@ -14071,10 +14041,10 @@
       <c r="LY11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="LZ11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA11" s="20" t="n">
+      <c r="LZ11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="MB11" s="19" t="n">
@@ -14140,10 +14110,10 @@
       <c r="MV11" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="MW11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX11" s="20" t="n">
+      <c r="MW11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX11" s="19" t="n">
         <v>0</v>
       </c>
       <c r="MY11" s="19" t="n">
@@ -14195,15 +14165,12 @@
         <v>0</v>
       </c>
       <c r="NO11" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP11" s="19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B12" s="11" t="n">
         <v>0</v>
@@ -14658,10 +14625,10 @@
       <c r="EV12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX12" s="12" t="n">
+      <c r="EW12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY12" s="11" t="n">
@@ -14730,10 +14697,10 @@
       <c r="FT12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV12" s="12" t="n">
+      <c r="FU12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW12" s="11" t="n">
@@ -14802,10 +14769,10 @@
       <c r="GR12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT12" s="12" t="n">
+      <c r="GS12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU12" s="11" t="n">
@@ -14862,10 +14829,10 @@
       <c r="HL12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN12" s="12" t="n">
+      <c r="HM12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO12" s="11" t="n">
@@ -14934,10 +14901,10 @@
       <c r="IJ12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL12" s="12" t="n">
+      <c r="IK12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM12" s="11" t="n">
@@ -15003,10 +14970,10 @@
       <c r="JG12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI12" s="12" t="n">
+      <c r="JH12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ12" s="11" t="n">
@@ -15069,10 +15036,10 @@
       <c r="KC12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE12" s="12" t="n">
+      <c r="KD12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF12" s="11" t="n">
@@ -15138,10 +15105,10 @@
       <c r="KZ12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB12" s="12" t="n">
+      <c r="LA12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC12" s="11" t="n">
@@ -15213,10 +15180,10 @@
       <c r="LY12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA12" s="12" t="n">
+      <c r="LZ12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB12" s="11" t="n">
@@ -15282,10 +15249,10 @@
       <c r="MV12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX12" s="12" t="n">
+      <c r="MW12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX12" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY12" s="11" t="n">
@@ -15337,15 +15304,12 @@
         <v>0</v>
       </c>
       <c r="NO12" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP12" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B13" s="11" t="n">
         <v>0</v>
@@ -15800,10 +15764,10 @@
       <c r="EV13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX13" s="12" t="n">
+      <c r="EW13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY13" s="11" t="n">
@@ -15872,10 +15836,10 @@
       <c r="FT13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV13" s="12" t="n">
+      <c r="FU13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW13" s="11" t="n">
@@ -15944,10 +15908,10 @@
       <c r="GR13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT13" s="12" t="n">
+      <c r="GS13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU13" s="11" t="n">
@@ -16004,10 +15968,10 @@
       <c r="HL13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN13" s="12" t="n">
+      <c r="HM13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO13" s="11" t="n">
@@ -16076,10 +16040,10 @@
       <c r="IJ13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL13" s="12" t="n">
+      <c r="IK13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM13" s="11" t="n">
@@ -16145,10 +16109,10 @@
       <c r="JG13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI13" s="12" t="n">
+      <c r="JH13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ13" s="11" t="n">
@@ -16211,10 +16175,10 @@
       <c r="KC13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE13" s="12" t="n">
+      <c r="KD13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF13" s="11" t="n">
@@ -16280,10 +16244,10 @@
       <c r="KZ13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB13" s="12" t="n">
+      <c r="LA13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC13" s="11" t="n">
@@ -16355,10 +16319,10 @@
       <c r="LY13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA13" s="12" t="n">
+      <c r="LZ13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB13" s="11" t="n">
@@ -16424,10 +16388,10 @@
       <c r="MV13" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX13" s="12" t="n">
+      <c r="MW13" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX13" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY13" s="11" t="n">
@@ -16479,15 +16443,12 @@
         <v>0</v>
       </c>
       <c r="NO13" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP13" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B14" s="11" t="n">
         <v>0</v>
@@ -16942,10 +16903,10 @@
       <c r="EV14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="EW14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="EX14" s="12" t="n">
+      <c r="EW14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="EX14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="EY14" s="11" t="n">
@@ -17014,10 +16975,10 @@
       <c r="FT14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="FU14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="FV14" s="12" t="n">
+      <c r="FU14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="FV14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="FW14" s="11" t="n">
@@ -17086,10 +17047,10 @@
       <c r="GR14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="GS14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="GT14" s="12" t="n">
+      <c r="GS14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="GT14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="GU14" s="11" t="n">
@@ -17146,10 +17107,10 @@
       <c r="HL14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="HM14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="HN14" s="12" t="n">
+      <c r="HM14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="HN14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="HO14" s="11" t="n">
@@ -17218,10 +17179,10 @@
       <c r="IJ14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="IK14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="IL14" s="12" t="n">
+      <c r="IK14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="IL14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="IM14" s="11" t="n">
@@ -17287,10 +17248,10 @@
       <c r="JG14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="JH14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="JI14" s="12" t="n">
+      <c r="JH14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="JJ14" s="11" t="n">
@@ -17353,10 +17314,10 @@
       <c r="KC14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="KD14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="KE14" s="12" t="n">
+      <c r="KD14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="KF14" s="11" t="n">
@@ -17422,10 +17383,10 @@
       <c r="KZ14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LA14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="LB14" s="12" t="n">
+      <c r="LA14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="LB14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="LC14" s="11" t="n">
@@ -17497,10 +17458,10 @@
       <c r="LY14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="LZ14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MA14" s="12" t="n">
+      <c r="LZ14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MA14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MB14" s="11" t="n">
@@ -17566,10 +17527,10 @@
       <c r="MV14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="MW14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="MX14" s="12" t="n">
+      <c r="MW14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="MY14" s="11" t="n">
@@ -17621,15 +17582,12 @@
         <v>0</v>
       </c>
       <c r="NO14" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="NP14" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
@@ -17782,8 +17740,8 @@
       <c r="ET15" s="22"/>
       <c r="EU15" s="22"/>
       <c r="EV15" s="22"/>
-      <c r="EW15" s="22"/>
-      <c r="EX15" s="23"/>
+      <c r="EW15" s="23"/>
+      <c r="EX15" s="22"/>
       <c r="EY15" s="22"/>
       <c r="EZ15" s="22"/>
       <c r="FA15" s="22"/>
@@ -17806,8 +17764,8 @@
       <c r="FR15" s="22"/>
       <c r="FS15" s="22"/>
       <c r="FT15" s="22"/>
-      <c r="FU15" s="22"/>
-      <c r="FV15" s="23"/>
+      <c r="FU15" s="23"/>
+      <c r="FV15" s="22"/>
       <c r="FW15" s="22"/>
       <c r="FX15" s="22"/>
       <c r="FY15" s="22"/>
@@ -17830,8 +17788,8 @@
       <c r="GP15" s="22"/>
       <c r="GQ15" s="22"/>
       <c r="GR15" s="22"/>
-      <c r="GS15" s="22"/>
-      <c r="GT15" s="23"/>
+      <c r="GS15" s="23"/>
+      <c r="GT15" s="22"/>
       <c r="GU15" s="22"/>
       <c r="GV15" s="22"/>
       <c r="GW15" s="22"/>
@@ -17850,8 +17808,8 @@
       <c r="HJ15" s="22"/>
       <c r="HK15" s="22"/>
       <c r="HL15" s="22"/>
-      <c r="HM15" s="22"/>
-      <c r="HN15" s="23"/>
+      <c r="HM15" s="23"/>
+      <c r="HN15" s="22"/>
       <c r="HO15" s="22"/>
       <c r="HP15" s="22"/>
       <c r="HQ15" s="22"/>
@@ -17874,8 +17832,8 @@
       <c r="IH15" s="22"/>
       <c r="II15" s="22"/>
       <c r="IJ15" s="22"/>
-      <c r="IK15" s="22"/>
-      <c r="IL15" s="23"/>
+      <c r="IK15" s="23"/>
+      <c r="IL15" s="22"/>
       <c r="IM15" s="22"/>
       <c r="IN15" s="22"/>
       <c r="IO15" s="22"/>
@@ -17897,8 +17855,8 @@
       <c r="JE15" s="22"/>
       <c r="JF15" s="22"/>
       <c r="JG15" s="22"/>
-      <c r="JH15" s="22"/>
-      <c r="JI15" s="23"/>
+      <c r="JH15" s="23"/>
+      <c r="JI15" s="22"/>
       <c r="JJ15" s="22"/>
       <c r="JK15" s="22"/>
       <c r="JL15" s="22"/>
@@ -17919,8 +17877,8 @@
       <c r="KA15" s="22"/>
       <c r="KB15" s="22"/>
       <c r="KC15" s="22"/>
-      <c r="KD15" s="22"/>
-      <c r="KE15" s="23"/>
+      <c r="KD15" s="23"/>
+      <c r="KE15" s="22"/>
       <c r="KF15" s="22"/>
       <c r="KG15" s="22"/>
       <c r="KH15" s="22"/>
@@ -17942,8 +17900,8 @@
       <c r="KX15" s="22"/>
       <c r="KY15" s="22"/>
       <c r="KZ15" s="22"/>
-      <c r="LA15" s="22"/>
-      <c r="LB15" s="23"/>
+      <c r="LA15" s="23"/>
+      <c r="LB15" s="22"/>
       <c r="LC15" s="22"/>
       <c r="LD15" s="22"/>
       <c r="LE15" s="22"/>
@@ -17967,8 +17925,8 @@
       <c r="LW15" s="22"/>
       <c r="LX15" s="22"/>
       <c r="LY15" s="22"/>
-      <c r="LZ15" s="22"/>
-      <c r="MA15" s="23"/>
+      <c r="LZ15" s="23"/>
+      <c r="MA15" s="22"/>
       <c r="MB15" s="22"/>
       <c r="MC15" s="22"/>
       <c r="MD15" s="22"/>
@@ -17990,8 +17948,8 @@
       <c r="MT15" s="22"/>
       <c r="MU15" s="22"/>
       <c r="MV15" s="22"/>
-      <c r="MW15" s="22"/>
-      <c r="MX15" s="23"/>
+      <c r="MW15" s="23"/>
+      <c r="MX15" s="22"/>
       <c r="MY15" s="22"/>
       <c r="MZ15" s="22"/>
       <c r="NA15" s="22"/>
@@ -18000,11 +17958,10 @@
       <c r="ND15" s="22"/>
       <c r="NE15" s="22"/>
       <c r="NF15" s="22"/>
-      <c r="NG15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
@@ -18157,8 +18114,8 @@
       <c r="ET16" s="22"/>
       <c r="EU16" s="22"/>
       <c r="EV16" s="22"/>
-      <c r="EW16" s="22"/>
-      <c r="EX16" s="23"/>
+      <c r="EW16" s="23"/>
+      <c r="EX16" s="22"/>
       <c r="EY16" s="22"/>
       <c r="EZ16" s="22"/>
       <c r="FA16" s="22"/>
@@ -18181,8 +18138,8 @@
       <c r="FR16" s="22"/>
       <c r="FS16" s="22"/>
       <c r="FT16" s="22"/>
-      <c r="FU16" s="22"/>
-      <c r="FV16" s="23"/>
+      <c r="FU16" s="23"/>
+      <c r="FV16" s="22"/>
       <c r="FW16" s="22"/>
       <c r="FX16" s="22"/>
       <c r="FY16" s="22"/>
@@ -18205,8 +18162,8 @@
       <c r="GP16" s="22"/>
       <c r="GQ16" s="22"/>
       <c r="GR16" s="22"/>
-      <c r="GS16" s="22"/>
-      <c r="GT16" s="23"/>
+      <c r="GS16" s="23"/>
+      <c r="GT16" s="22"/>
       <c r="GU16" s="22"/>
       <c r="GV16" s="22"/>
       <c r="GW16" s="22"/>
@@ -18225,8 +18182,8 @@
       <c r="HJ16" s="22"/>
       <c r="HK16" s="22"/>
       <c r="HL16" s="22"/>
-      <c r="HM16" s="22"/>
-      <c r="HN16" s="23"/>
+      <c r="HM16" s="23"/>
+      <c r="HN16" s="22"/>
       <c r="HO16" s="22"/>
       <c r="HP16" s="22"/>
       <c r="HQ16" s="22"/>
@@ -18249,8 +18206,8 @@
       <c r="IH16" s="22"/>
       <c r="II16" s="22"/>
       <c r="IJ16" s="22"/>
-      <c r="IK16" s="22"/>
-      <c r="IL16" s="23"/>
+      <c r="IK16" s="23"/>
+      <c r="IL16" s="22"/>
       <c r="IM16" s="22"/>
       <c r="IN16" s="22"/>
       <c r="IO16" s="22"/>
@@ -18272,8 +18229,8 @@
       <c r="JE16" s="22"/>
       <c r="JF16" s="22"/>
       <c r="JG16" s="22"/>
-      <c r="JH16" s="22"/>
-      <c r="JI16" s="23"/>
+      <c r="JH16" s="23"/>
+      <c r="JI16" s="22"/>
       <c r="JJ16" s="22"/>
       <c r="JK16" s="22"/>
       <c r="JL16" s="22"/>
@@ -18294,8 +18251,8 @@
       <c r="KA16" s="22"/>
       <c r="KB16" s="22"/>
       <c r="KC16" s="22"/>
-      <c r="KD16" s="22"/>
-      <c r="KE16" s="23"/>
+      <c r="KD16" s="23"/>
+      <c r="KE16" s="22"/>
       <c r="KF16" s="22"/>
       <c r="KG16" s="22"/>
       <c r="KH16" s="22"/>
@@ -18317,8 +18274,8 @@
       <c r="KX16" s="22"/>
       <c r="KY16" s="22"/>
       <c r="KZ16" s="22"/>
-      <c r="LA16" s="22"/>
-      <c r="LB16" s="23"/>
+      <c r="LA16" s="23"/>
+      <c r="LB16" s="22"/>
       <c r="LC16" s="22"/>
       <c r="LD16" s="22"/>
       <c r="LE16" s="22"/>
@@ -18342,8 +18299,8 @@
       <c r="LW16" s="22"/>
       <c r="LX16" s="22"/>
       <c r="LY16" s="22"/>
-      <c r="LZ16" s="22"/>
-      <c r="MA16" s="23"/>
+      <c r="LZ16" s="23"/>
+      <c r="MA16" s="22"/>
       <c r="MB16" s="22"/>
       <c r="MC16" s="22"/>
       <c r="MD16" s="22"/>
@@ -18365,8 +18322,8 @@
       <c r="MT16" s="22"/>
       <c r="MU16" s="22"/>
       <c r="MV16" s="22"/>
-      <c r="MW16" s="22"/>
-      <c r="MX16" s="23"/>
+      <c r="MW16" s="23"/>
+      <c r="MX16" s="22"/>
       <c r="MY16" s="22"/>
       <c r="MZ16" s="22"/>
       <c r="NA16" s="22"/>
@@ -18375,7 +18332,6 @@
       <c r="ND16" s="22"/>
       <c r="NE16" s="22"/>
       <c r="NF16" s="22"/>
-      <c r="NG16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24"/>
@@ -21340,7 +21296,7 @@
       <c r="A1003" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="100">
+  <mergeCells count="99">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:K1"/>
@@ -21380,69 +21336,68 @@
     <mergeCell ref="EE1:EH1"/>
     <mergeCell ref="EJ1:EN1"/>
     <mergeCell ref="EP1:ER1"/>
-    <mergeCell ref="EV1:EW1"/>
-    <mergeCell ref="EY1:FA1"/>
-    <mergeCell ref="FC1:FG1"/>
-    <mergeCell ref="FJ1:FK1"/>
-    <mergeCell ref="FN1:FO1"/>
-    <mergeCell ref="FQ1:FR1"/>
-    <mergeCell ref="FT1:FV1"/>
-    <mergeCell ref="FW1:FX1"/>
-    <mergeCell ref="FY1:GB1"/>
-    <mergeCell ref="GD1:GG1"/>
-    <mergeCell ref="GH1:GK1"/>
-    <mergeCell ref="GM1:GN1"/>
-    <mergeCell ref="GP1:GQ1"/>
-    <mergeCell ref="GS1:GT1"/>
-    <mergeCell ref="GW1:GY1"/>
-    <mergeCell ref="GZ1:HA1"/>
-    <mergeCell ref="HC1:HE1"/>
-    <mergeCell ref="HF1:HH1"/>
-    <mergeCell ref="HL1:HN1"/>
-    <mergeCell ref="HO1:HQ1"/>
-    <mergeCell ref="HS1:HT1"/>
-    <mergeCell ref="HU1:HV1"/>
-    <mergeCell ref="HY1:IB1"/>
-    <mergeCell ref="IC1:IF1"/>
-    <mergeCell ref="IG1:II1"/>
-    <mergeCell ref="IK1:IL1"/>
-    <mergeCell ref="IM1:IP1"/>
-    <mergeCell ref="IR1:IV1"/>
-    <mergeCell ref="IX1:IY1"/>
-    <mergeCell ref="JA1:JB1"/>
-    <mergeCell ref="JE1:JF1"/>
-    <mergeCell ref="JJ1:JL1"/>
-    <mergeCell ref="JN1:JO1"/>
-    <mergeCell ref="JT1:JU1"/>
-    <mergeCell ref="JW1:JZ1"/>
-    <mergeCell ref="KA1:KC1"/>
-    <mergeCell ref="KG1:KI1"/>
-    <mergeCell ref="KK1:KM1"/>
-    <mergeCell ref="KP1:KS1"/>
-    <mergeCell ref="KX1:KZ1"/>
-    <mergeCell ref="LC1:LF1"/>
-    <mergeCell ref="LG1:LH1"/>
-    <mergeCell ref="LI1:LJ1"/>
-    <mergeCell ref="LL1:LM1"/>
-    <mergeCell ref="LN1:LQ1"/>
-    <mergeCell ref="LS1:LT1"/>
-    <mergeCell ref="LV1:LW1"/>
-    <mergeCell ref="LZ1:MA1"/>
-    <mergeCell ref="MB1:MD1"/>
-    <mergeCell ref="MH1:MI1"/>
-    <mergeCell ref="MJ1:MK1"/>
-    <mergeCell ref="ML1:MM1"/>
-    <mergeCell ref="MO1:MP1"/>
-    <mergeCell ref="MR1:MT1"/>
-    <mergeCell ref="MU1:MV1"/>
-    <mergeCell ref="MY1:MZ1"/>
-    <mergeCell ref="NA1:NB1"/>
-    <mergeCell ref="NF1:NG1"/>
-    <mergeCell ref="NH1:NJ1"/>
-    <mergeCell ref="NK1:NN1"/>
-    <mergeCell ref="NO1:NP1"/>
+    <mergeCell ref="EX1:EZ1"/>
+    <mergeCell ref="FB1:FF1"/>
+    <mergeCell ref="FI1:FJ1"/>
+    <mergeCell ref="FM1:FN1"/>
+    <mergeCell ref="FP1:FQ1"/>
+    <mergeCell ref="FS1:FU1"/>
+    <mergeCell ref="FV1:FW1"/>
+    <mergeCell ref="FX1:GA1"/>
+    <mergeCell ref="GC1:GF1"/>
+    <mergeCell ref="GG1:GJ1"/>
+    <mergeCell ref="GL1:GM1"/>
+    <mergeCell ref="GO1:GP1"/>
+    <mergeCell ref="GR1:GS1"/>
+    <mergeCell ref="GV1:GX1"/>
+    <mergeCell ref="GY1:GZ1"/>
+    <mergeCell ref="HB1:HD1"/>
+    <mergeCell ref="HE1:HG1"/>
+    <mergeCell ref="HK1:HM1"/>
+    <mergeCell ref="HN1:HP1"/>
+    <mergeCell ref="HR1:HS1"/>
+    <mergeCell ref="HT1:HU1"/>
+    <mergeCell ref="HX1:IA1"/>
+    <mergeCell ref="IB1:IE1"/>
+    <mergeCell ref="IF1:IH1"/>
+    <mergeCell ref="IJ1:IK1"/>
+    <mergeCell ref="IL1:IO1"/>
+    <mergeCell ref="IQ1:IU1"/>
+    <mergeCell ref="IW1:IX1"/>
+    <mergeCell ref="IZ1:JA1"/>
+    <mergeCell ref="JD1:JE1"/>
+    <mergeCell ref="JI1:JK1"/>
+    <mergeCell ref="JM1:JN1"/>
+    <mergeCell ref="JS1:JT1"/>
+    <mergeCell ref="JV1:JY1"/>
+    <mergeCell ref="JZ1:KB1"/>
+    <mergeCell ref="KF1:KH1"/>
+    <mergeCell ref="KJ1:KL1"/>
+    <mergeCell ref="KO1:KR1"/>
+    <mergeCell ref="KW1:KY1"/>
+    <mergeCell ref="LB1:LE1"/>
+    <mergeCell ref="LF1:LG1"/>
+    <mergeCell ref="LH1:LI1"/>
+    <mergeCell ref="LK1:LL1"/>
+    <mergeCell ref="LM1:LP1"/>
+    <mergeCell ref="LR1:LS1"/>
+    <mergeCell ref="LU1:LV1"/>
+    <mergeCell ref="LY1:LZ1"/>
+    <mergeCell ref="MA1:MC1"/>
+    <mergeCell ref="MG1:MH1"/>
+    <mergeCell ref="MI1:MJ1"/>
+    <mergeCell ref="MK1:ML1"/>
+    <mergeCell ref="MN1:MO1"/>
+    <mergeCell ref="MQ1:MS1"/>
+    <mergeCell ref="MT1:MU1"/>
+    <mergeCell ref="MX1:MY1"/>
+    <mergeCell ref="MZ1:NA1"/>
+    <mergeCell ref="NE1:NF1"/>
+    <mergeCell ref="NG1:NI1"/>
+    <mergeCell ref="NJ1:NM1"/>
+    <mergeCell ref="NN1:NO1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:NP14">
+  <conditionalFormatting sqref="B3:NO14">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>